<commit_message>
Giải thích hóa lộc ở các cung
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tuvi\TuVi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61090875-EF96-444F-84A5-1F983B9C2985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD416E2-BDDC-4322-BD64-7DEA5148560C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3290" uniqueCount="1844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3298" uniqueCount="1852">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -5567,6 +5567,30 @@
   </si>
   <si>
     <t>Vị trí cung Điền Trạch so với ngũ hành Mệnh: Bại địa</t>
+  </si>
+  <si>
+    <t>Trường hợp cung điền trạch có Hóa Lộc, thông thường sau khi mệnh tạo sinh ra, gia vận bỗng nhiên chuyển biến tốt lên, tình trạng cha mẹ và kinh tế trong nhà đều được nâng cao, khiến mệnh tạo có hoàn cảnh học hành khá tốt. Vì cung điền trạch là cung vị biểu hiện của nơi sâu thẳm nhất trong tâm hồn, nên trường hợp cung điền trạch có Hóa Lộc là chủ về mệnh tạo bộc lộ toàn bộ tính đa tình và hòa hợp của mình, đối với cách xử lí mọi việc đều cầu hài hòa.</t>
+  </si>
+  <si>
+    <t>Vì Hóa Lộc có xu thế là "nhiều", do đó, thường thường mệnh tạo sẽ có nhiều bất động sản, đồng thời trong nhà có rất nhiều đồ đạc. Hóa Lộc cũng chủ về thích xa hoa, vì vậy nơi cư trú của mệnh tạo thường thường được trang hoàng rất hoa lệ, sang trọng, hoặc ít nhất cũng phải có thẩm mĩ. Cung điền trạch còn chủ về gia đình, vì Hóa Lộc ở cung điền trạch cho nên nơi mệnh tạo đặt kì vọng là gia đình, và mệnh tạo cũng trông mong người nhà đối xử với nhau hòa hợp, hi vọng có thể "hòa khí sinh tài". Lúc cung điền trạch chủ về gia đình, cũng nên xem xét đối cung của nó là cung tử nữ. Có Hóa Lộc là chủ về con cái hướng về gia đình, gia đình là nơi con cái có cảm giác ấm áp, ngọt ngào.</t>
+  </si>
+  <si>
+    <t>Thường thường hoàn cảnh gia đình khá tốt, có tiền, có nhiều bất động sản, nhưng nếu vị trí Hóa Kị [năm sinh] không thích đáng, sẽ xảy ra tình hình "Lộc đi theo Kị", e rằng sẽ không giữ được bất động sản.  Hóa Lộc còn sợ bị xung, trường hợp cung điền trạch có Hóa Lộc, mà Hóa Kị không ở "ngã cung", thì cung điền trạch nên có thêm Hóa Quyền hoặc Hóa Khoa, dù gặp xung, cũng có thể giữ được chút "lộc".</t>
+  </si>
+  <si>
+    <t>Vì cung điền trạch là cung vị tổng "thu vào", Hóa Lộc ở cung vị chủ về tổng "thu vào", nên phần nhiều mệnh tạo sẽ có thói quen thu thập mọi thứ.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch còn chủ về môi trường làm việc, trường hợp Hóa Lộc ở cung điền trạch, là làm việc nhiều công ti, hoặc thay đổi công việc nhiều lần. Vì có Hóa Lộc, cho nên bất luận nhận chức ở công ti có vốn liếng hùng hậu hay không, cũng đều chủ về có tình cảm hòa hợp ở nơi làm việc, cũng không loại trừ tình huống đông sự đối xử rất tốt với mệnh tạo.</t>
+  </si>
+  <si>
+    <t>Tuyến "tử điền" phần nhiều chủ về đào hoa, hưởng lạc. Lúc luận về đào hoa, cung tử nữ có thể đại biểu cho đối tượng đào hoa; trường hợp Hóa Lộc ở cung điền trạch là chủ về đối tượng đào hoa có hảo cảm với gia đình của mệnh tạo, mong muốn thành thành viên của gia đình, hoặc đối tượng đào hoa dòm ngó sản nghiệp của mệnh tạo, mà đối tượng đào hoa là người đa tình, xử sự theo cảm tính. Cung điền trạch có Hóa Lộc có thể dẫn đến cơ hội đào hoa sau khi kết hôn.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch còn là cung vị biểu hiện của cung tật ách, có thể tượng trưng cho y liệu; lúc mệnh tạo bị bệnh phần nhiều đều có thái độ đối mặt rất lạc quan, tích cực; nhưng không có nghĩa là không nguy hiểm. Vì Hóa Lộc có hàm nghĩa là "nhiều", nên mệnh tạo thường đi nhiều nơi để chữa trị.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch còn là cung vị phu thê của cung nô bộc, ý ở đây là sẽ có những người phối ngẫu của bạn bè (bao gồm những người chưa quen biết) có cơ hội "vào" gia đình của mệnh tạo, muốn trở thành một thành viên trong nhà của mệnh tạo; cho nên, mệnh tạo có nhiều cơ hội quen biết với những người đã có hôn ước.</t>
   </si>
 </sst>
 </file>
@@ -5914,10 +5938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:G1635"/>
+  <dimension ref="A2:J1635"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1626" workbookViewId="0">
-      <selection activeCell="B1635" sqref="B1635"/>
+    <sheetView tabSelected="1" topLeftCell="A1176" workbookViewId="0">
+      <selection activeCell="D1177" sqref="D1177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5925,6 +5949,12 @@
     <col min="1" max="2" width="44.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="56.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -11145,7 +11175,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="653" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A653" s="1" t="s">
         <v>682</v>
       </c>
@@ -15273,7 +15303,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="1169" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1169" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1169" s="1" t="s">
         <v>1195</v>
       </c>
@@ -15281,7 +15311,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="1170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1170" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1170" s="1" t="s">
         <v>9</v>
       </c>
@@ -15289,7 +15319,7 @@
         <v>1832</v>
       </c>
     </row>
-    <row r="1171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1171" s="1" t="s">
         <v>10</v>
       </c>
@@ -15297,7 +15327,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1172" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1172" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1172" s="1" t="s">
         <v>11</v>
       </c>
@@ -15305,7 +15335,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="1173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1173" s="1" t="s">
         <v>12</v>
       </c>
@@ -15313,7 +15343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1174" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1174" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1174" s="1" t="s">
         <v>13</v>
       </c>
@@ -15321,7 +15351,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="1175" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="1175" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A1175" s="1" t="s">
         <v>14</v>
       </c>
@@ -15329,7 +15359,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="1176" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="1176" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A1176" s="1" t="s">
         <v>15</v>
       </c>
@@ -15340,15 +15370,39 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="1177" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="1177" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A1177" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1177" s="1" t="s">
         <v>1744</v>
       </c>
-    </row>
-    <row r="1178" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="C1177" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="D1177" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="E1177" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="F1177" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="G1177" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="H1177" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="I1177" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="J1177" s="1" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A1178" s="1" t="s">
         <v>17</v>
       </c>
@@ -15359,7 +15413,7 @@
         <v>1746</v>
       </c>
     </row>
-    <row r="1179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1179" s="1" t="s">
         <v>18</v>
       </c>
@@ -15367,7 +15421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1180" s="1" t="s">
         <v>19</v>
       </c>
@@ -15375,7 +15429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="1181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1181" s="1" t="s">
         <v>20</v>
       </c>
@@ -15383,7 +15437,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1182" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1182" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1182" s="1" t="s">
         <v>21</v>
       </c>
@@ -15391,7 +15445,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="1183" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="1183" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A1183" s="1" t="s">
         <v>22</v>
       </c>
@@ -15399,7 +15453,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="1184" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1184" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1184" s="1" t="s">
         <v>23</v>
       </c>
@@ -19107,7 +19161,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="1633" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1633" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1633" s="1" t="s">
         <v>1841</v>
       </c>
@@ -19123,7 +19177,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="1635" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1635" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1635" s="1" t="s">
         <v>1843</v>
       </c>

</xml_diff>

<commit_message>
Giải thích hóa quyền tại phụ mẫu
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD416E2-BDDC-4322-BD64-7DEA5148560C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DBAD42-1D61-45BC-8B0B-5EADB0F60DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3298" uniqueCount="1852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="1860">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -5591,6 +5591,30 @@
   </si>
   <si>
     <t>Cung điền trạch còn là cung vị phu thê của cung nô bộc, ý ở đây là sẽ có những người phối ngẫu của bạn bè (bao gồm những người chưa quen biết) có cơ hội "vào" gia đình của mệnh tạo, muốn trở thành một thành viên trong nhà của mệnh tạo; cho nên, mệnh tạo có nhiều cơ hội quen biết với những người đã có hôn ước.</t>
+  </si>
+  <si>
+    <t>Hóa Quyền chủ về lực hành động và lực lôi kéo mạnh mẽ; còn cung điền trạch là đại biểu cho bất động sản, đương nhiên sẽ khiến mệnh tạo rất muốn có bất động sản, tử đó sẽ có ý muốn mua nhà rất mạnh, khiến mệnh tạo tất bật làm việc, miệt mài giành dụm tiền đế mua bất động sản, luôn luôn có tâm lí muốn có nhiều. Cung điền trạch có Hóa Quyền thường thường cũng chủ về có nhiều bất động sản. Hóa Quyền có xu thế thay đổi mau lẹ, do đó mệnh tạo rất dễ thay đổi bất động sản; hơn nữa, như đã thuật ở trước, mệnh tạo sẽ không ngừng có ý muốn mua bất động sản, họ thường dùng bất động sản làm công cụ quản lí tiền bạc và cũng là phương thức kiếm tiền. Điền trạch là cung vị biểu hiện của chỗ sâu thẳm trong tâm hồn (cung tật ách), trường hợp cung điền trạch xuất hiện Hóa Quyền, là từ nơi sâu thẳm trong tâm hồn sẽ bộc lộ với thế quá mạnh, lúc gặp tình huống bộc phát đột ngột (lúc đại vận khơi động cung tật ách), mệnh tạo sẽ lộ rõ tính hấp tấp, dễ bị kích động, vội vàng, dê có thái độ bức bách người khác, lúc bình thường phần nhiều họ sẽ rất thích làm chủ đạo, thích ép buộc người khác.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch là cung vị biểu hiện của cung tật ách, do đó có thể tượng trưng cho y liệu; trường hợp Hóa Quyền ở cung điền trạch, thường thường lúc mệnh tạo đối mặt với bệnh tật, sẽ rất tích cực chữa trị, cũng thường hay đối bác sĩ, thầy thuốc, hoặc thử nhiều liệu pháp khác nhau; nhưng phân tích tỉ mỉ thì thấy thái độ của mệnh tạo không lạc quan, mà lại dễ bị kích động, vội vàng khi đối diện với mọi vấn đề. Trường hợp Hóa Quyền ở cung điền trạch, trước tiên có thể nghĩ đến là, trong lòng mệnh tạo hay lo lắng không yên, khó tâm bình khí hòa. Vì cung điền trạch còn là cung vị chủ về bệnh tật, nên mệnh tạo dễ mắc nhiều bệnh chứng khác nhau, thường thường sức khỏe biến đổi rất nhanh, lúc phát bệnh dễ gặp tình huống kịch liệt.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch còn có thể chủ về quan hệ của cả gia đình, trường hợp cung điền trạch có Hóa Quyền, mệnh tạo là người nắm quyền trong nhà, đối với chuyện lớn nhỏ trong nhà đều là người quyết định, có sức ảnh hưởng tuyệt đối. Nhưng vì lực tác động của Hóa Quyền là đến thẳng đi thẳng, và nghiêm túc, vì vậy tuy mệnh tạo và người nhà cư xử với nhau tốt đẹp (vì Hóa Quyền chủ vẻ qua lại dồn dập), nhưng lại thiếu cảm giác ấm áp.</t>
+  </si>
+  <si>
+    <t>Trước đã đề cập Hóa Quyền chủ về biến động, không ổn định, trường hợp Hóa Quyền ở cung điền trạch, còn chủ về mệnh tạo ít ở nhà, thường hay ở bên ngoài. Xét ở góc độ khác, khách đến nhà mệnh tạo cũng nhiều, tình huống biến động khá nhanh. Nếu dùng cung điền trạch để xem về gia đình, có Hóa Quyền, đối với con cái sẽ có hai ý nghĩa. Một là, vì cung vị thiên di cua cung tử nữ có Hóa Quyền, sẽ dễ có "dịch động" và lí tưởng cao; hai là, bất luận "dịch động" như thế nào, đối với chúng, gia đình trước sau vẫn là quan trọng nhất, cho nên trong cả gia tộc, lực hướng tâm của con cái cực mạnh.</t>
+  </si>
+  <si>
+    <t>Nếu lấy Hóa Quyền để luận đoán hình tượng, nội dung, trường hợp Hóa Quyền ở cung điền trạch, phần nhiều nhà ở của mệnh tạo đều có cách cục chỉnh tề, có khí thế, nội thất có nhiều thiết bị cứng, toàn thể hoàn cảnh cư trú khá tốt.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch còn là cung vị tổng thu tóm vào bên trong, cho nên cùng giống như Hóa Lộc ở cung điền trạch, cá tính hay chỗ thâm sâu nhất của tâm hồn mệnh tạo sẽ khiến họ có thói quen thu thập, sưu tập thứ gì đó, nhưng vì Hóa Quyền, mệnh tạo sẽ dễ có tính xung động nhất thời, sẽ thường thay đổi thể loại sưu tập hoặc đồ vật thích thu thập.</t>
+  </si>
+  <si>
+    <t>Nếu lấy cung điền trạch để chủ về môi trường làm việc, trường hợp Hóa Quyền ở cung điền trạch, là chủ về công ti mệnh tạo làm việc rất có lực cạnh tranh trong giới làm ăn. Nhưng xem xét ở góc độ khác, mệnh tạo ở trong môi trường làm việc cũng thường xuyên phải đối diện với sự khiêu chiến và cạnh tranh, công nhân viên chức của nội bộ công ti cũng sẽ thay đổi liên tục.</t>
+  </si>
+  <si>
+    <t>rong tiết bàn về trường hợp cung điền trạch có Hóa Lộc [năm sinh], chứng tôi đã đê cập vấn đề tứ hóa ở tuyến "tử điền" phần nhiều có dính đến đào hoa; Hóa Quyền ở cung điền trạch cũng làm tăng khả năng có đào hoa. Còn vì lực tác động của Hóa Quyền là ép buộc, mau lẹ, nhất thời, do đó khiến cho người ta cảm thấy khó chống lại hơn, dễ rơi vào quan hệ đào hoa hơn so với trường hợp đào hoa của Hóa Lộc; hơn nữa, có thể sau khi kết hôn mới xảy ra cơ hội.</t>
   </si>
 </sst>
 </file>
@@ -5938,10 +5962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:J1635"/>
+  <dimension ref="A2:K1635"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1176" workbookViewId="0">
-      <selection activeCell="D1177" sqref="D1177"/>
+    <sheetView tabSelected="1" topLeftCell="E1177" workbookViewId="0">
+      <selection activeCell="J1178" sqref="J1178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5955,6 +5979,7 @@
     <col min="8" max="8" width="30.7109375" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" customWidth="1"/>
     <col min="10" max="10" width="36.7109375" customWidth="1"/>
+    <col min="11" max="11" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -15303,7 +15328,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="1169" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1169" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1169" s="1" t="s">
         <v>1195</v>
       </c>
@@ -15311,7 +15336,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="1170" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1170" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1170" s="1" t="s">
         <v>9</v>
       </c>
@@ -15319,7 +15344,7 @@
         <v>1832</v>
       </c>
     </row>
-    <row r="1171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1171" s="1" t="s">
         <v>10</v>
       </c>
@@ -15327,7 +15352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1172" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1172" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1172" s="1" t="s">
         <v>11</v>
       </c>
@@ -15335,7 +15360,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="1173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1173" s="1" t="s">
         <v>12</v>
       </c>
@@ -15343,7 +15368,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1174" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1174" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1174" s="1" t="s">
         <v>13</v>
       </c>
@@ -15351,7 +15376,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="1175" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="1175" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1175" s="1" t="s">
         <v>14</v>
       </c>
@@ -15359,7 +15384,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="1176" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="1176" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A1176" s="1" t="s">
         <v>15</v>
       </c>
@@ -15370,7 +15395,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="1177" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+    <row r="1177" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A1177" s="1" t="s">
         <v>16</v>
       </c>
@@ -15402,7 +15427,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="1178" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="1178" spans="1:11" ht="285" x14ac:dyDescent="0.25">
       <c r="A1178" s="1" t="s">
         <v>17</v>
       </c>
@@ -15412,8 +15437,32 @@
       <c r="C1178" s="1" t="s">
         <v>1746</v>
       </c>
-    </row>
-    <row r="1179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D1178" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="E1178" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="F1178" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="G1178" s="1" t="s">
+        <v>1855</v>
+      </c>
+      <c r="H1178" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="I1178" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="J1178" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="K1178" s="1" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1179" s="1" t="s">
         <v>18</v>
       </c>
@@ -15421,7 +15470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1180" s="1" t="s">
         <v>19</v>
       </c>
@@ -15429,7 +15478,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="1181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1181" s="1" t="s">
         <v>20</v>
       </c>
@@ -15437,7 +15486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1182" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1182" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1182" s="1" t="s">
         <v>21</v>
       </c>
@@ -15445,7 +15494,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="1183" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="1183" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A1183" s="1" t="s">
         <v>22</v>
       </c>
@@ -15453,7 +15502,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="1184" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1184" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1184" s="1" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Gảii thích hoàn thiện tứ hóa 12 cung
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DBAD42-1D61-45BC-8B0B-5EADB0F60DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03600D6E-6A47-45F7-88DC-69CE3AFC32B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="1860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="1880">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -5615,6 +5615,66 @@
   </si>
   <si>
     <t>rong tiết bàn về trường hợp cung điền trạch có Hóa Lộc [năm sinh], chứng tôi đã đê cập vấn đề tứ hóa ở tuyến "tử điền" phần nhiều có dính đến đào hoa; Hóa Quyền ở cung điền trạch cũng làm tăng khả năng có đào hoa. Còn vì lực tác động của Hóa Quyền là ép buộc, mau lẹ, nhất thời, do đó khiến cho người ta cảm thấy khó chống lại hơn, dễ rơi vào quan hệ đào hoa hơn so với trường hợp đào hoa của Hóa Lộc; hơn nữa, có thể sau khi kết hôn mới xảy ra cơ hội.</t>
+  </si>
+  <si>
+    <t>Trường hợp cung điền trạch thấy Hóa Khoa, là chủ về mệnh tạo có năng lực quản lí tiền bạc, sử dụng tài sản, bất động sản hợp lí, là nhân tài quản lí tài sản và quy hoạch bất động sản. Vì Hóa Khoa có tác dụng kéo dài, tăng sự vững bền, cho nên cách quản lí tiền bạc và năng lực quy hoạch bất động sản của họ cũng thuộc loại có kế hoạch lâu dài.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Do lực tác động của Hóa Khoa ở trong cung điền trạch là vãn hồi, giải nguy, cho nên tài sản của mệnh tạo được bảo vệ, tiền bạc thường lúc nào cũng có, mệnh tạo còn có thói quen giữ tiền riêng, năng lực giữ tiền cực tốt.</t>
+  </si>
+  <si>
+    <t>Nhưng Hóa Khoa ở cung điền trạch, không nhất định sẽ giữ được mãi bất động sản, mà phải xem cung tật ách (cung vị khí số của cung điền trạch) để định. Vì có Hóa Khoa, nên dù bị phá sản hay bất động sản bị tổn thất, vẫn có thể giấu riêng được một số của cải. Lúc xem cung điền trạch là thực thế bất động sản, thấy có Hóa Khoa, là chủ về nhà ở trang hoàng, bài trí thanh nhã, trong nhà lúc nào cũng sạch sẽ, chỉnh tề, nhưng không phải trang trí kiểu khoa trương hào nhoáng theo thói tục, ý tứ rất tinh xảo.</t>
+  </si>
+  <si>
+    <t>Ý tượng của cung điền trạch còn có thể suy rộng ra thành các tình huống cuộc sống của những trong người nhà; trường hợp có Hóa Khoa, có thể đoán mệnh tạo và người nhà sống với nhau hòa hợp vui vẻ; nhà ở hiếm khi bị trộm cướp, hỏa tai, rò rỉ nước; hơn nữa, còn có thể sống hòa mục với xóm giềng. Cung điền trạch là cung vị tài bạch của cung tật ách, có thể xem là cung vị biểu hiện của tầng thâm sâu trong tâm hồn, thấy Hóa Khoa là mẫu người lí trí; dù bề ngoài trông giống như người xấu, hoặc tính khi có vẻ như không được tốt lắm, nhưng họ là người mặt ác mà tâm thiện.</t>
+  </si>
+  <si>
+    <t>Do có lực tác động của Hóa Khoa [năm sinh] ở trong cung điền trạch, nếu gặp lúc không thuận lợi, có thể lợi dụng thời gian ở nhà để tâm tình được trầm lắng, có thể nhờ từ trường và sức ảnh hưởng của gia đình mà ngộ ra cách giải quyết vấn đề (cũng có thể dựa vào việc chính đốn việc nhà mà nghĩ ra được biện pháp tốt).</t>
+  </si>
+  <si>
+    <t>Xét ở góc độ bệnh tật, tai ách, cung điền trạch là chủ về phụ khoa, cơ quan trong cơ thể phụ nữ như tử cung và buồng trứng; thấy Hóa Khoa, là chủ về ít khi gặp các vấn đề về bệnh phụ khoa, sinh đẻ. Cùng vì cung điền trạch là cung vị biểu hiện của cung tật ách, trường hợp có Hóa Khoa nhập cung điền trạch, là chủ về lúc mệnh tạo bị tai nạn hay bệnh tật, thường thường đều được thầy giỏi thuốc hay chữa trị kịp thời.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xét từ góc độ con cái, cung điền trạch là cung vị thiên di của cung tử nữ, trường hợp có Hóa Khoa, là con cái rất hướng về gia đình, cho rằng gia đình là nơi bảo vệ chúng, là nơi con cái đặt kì vọng, nên luôn duy trì mối ràng buộc hòa hợp với gia đình.</t>
+  </si>
+  <si>
+    <t>Xét ở góc độ cha mẹ, cung điền trạch là cung vị phúc đức của cung phụ mẫu, trường hợp có Hóa Khoa, là chủ về quan hệ hôn nhằn của cha mẹ rất hòa hợp, gia đình của mệnh tạo có cuộc sống yên ổn vui vẻ.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch còn đại biểu cho môi trường làm việc, cho nên trường hợp Hóa Khoa ở cung điền trạch, là chủ về môi trường làm việc rất vững chắc, là co cấu nổi tiếng hoặc có hình tượng tốt đẹp trong xã hội.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch là cung vị tật ách của cung tài bạch, liên quan đến ý niệm ở tầng sâu thẳm nhất trong tâm hồn về phương cách kiếm tiền, đồng thời còn có ý tượng là "kho tài bạch". Trường hợp cung điền trạch có Hóa Kị, là ý thức về nguy cơ có kiếm được tiền liên tục hay không, bản thân thiếu cảm giác an toàn về tài phú; là người nặng tư duy thực dụng. Vì cung điền trạch là "ngã cung", có Hóa Kị là chủ về không ra ngoài, biểu hiện trong cuộc sống thường nhật là mệnh tạo sẽ giấu tiền riêng để chi dụng trong lúc cần kíp.</t>
+  </si>
+  <si>
+    <t>Tiếp theo trên, tuy mệnh tạo lúc nào cũng có cảm giác không an toàn về tiền bạc, nhưng vì quan hệ nhân quả đối ứng của Hóa Lộc và Hóa Kị, nếu Hóa Lộc [năm sinh] ở "ngã cung", mệnh tạo sẽ vì cảm giác không an toàn này mà liều mạng kiếm tiền, quyết tâm tích lũy tiền bạc, có tiềm lực làm cho gia sản trở nên to tát. Nếu Hóa Lộc [năm sinh] ở "tha cung", tuy muốn có nhiều tài phú, nhưng thường thường là trái với ý nguyện, sẽ vì đầu tư sai lầm mà hao tốn "kho tiền". Cho nên có Hóa Lộc [năm sinh] ở "tha cung", là người mê tiền của nhưng không giỏi quản lí tiền của.</t>
+  </si>
+  <si>
+    <t>Nếu đối góc độ xem xét, thì cung điền trạch là đại biểu hiện cho nơi sâu thẳm nhất trong tâm hồn; trường hợp cung điền trạch có Hóa Kị, là nơi sâu thẳm nhất trong tâm hồn có biểu hiện không được tốt, tình huống thực tế là mệnh tạo thường dùng mưu kế và tiểu xảo, lúc gặp sự cố xảy ra đột ngột sẽ có phản ứng sai lầm, thậm chí dễ nổi giận.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch còn tượng trưng cho hoàn cảnh nhà ở; trường hợp cung điền trạch có Hóa Kị, vì Hóa Kị có ý tượng là "thu vào", còn có ý tượng "bừa bộn, ngổn ngang", nên trong nhà dễ thấy bừa bộn, ngổn ngang; truy cứu nguyên nhân, phần nhiều là vì mệnh tạo mua hay sưu tập rất nhiều đồ đạc, gia cụ vật phẩm, mà xếp đặt bài trí rất lộn xộn; còn có thói quen thanh lí đồ linh tinh theo kiểu bỏ mà không vứt đi, ngay cả phòng khách được sửa sang sạch sẽ nhưng lại giống như gian phòng chứa đồ vật linh tinh, nếu không có sự chuẩn bị tâm lí đế mở cửa bước vào, bạn sẽ có cảm giác ở đây từng là bãi chiến trường.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch cũng có thể xem về bất động sản do mệnh tạo mua tậu được; trường hợp cung điền trạch có Hóa Kị, là chủ về mệnh tạo có bất động sản nhưng quyền sở hữu không rõ ràng (hai ba người cùng đứng tên ..) hoặc có tình trạng chuyển dời bất động sản rất phiền phức, mà bất động sản còn dễ bị rò rỉ nước, đường ống nước không thông ... Nếu có các hung tinh như Hỏa Tinh, Linh Tinh, Thiên Hình thì dễ bị trộm cướp hay hỏa tai.</t>
+  </si>
+  <si>
+    <t>Nó còn là cung vị biểu hiện của cung tật ách, là biểu hiện của nơi sâu thẳm nhất trong tâm hồn, và còn dùng để luận giải bệnh tật; trường hợp có Hóa Kị, một là chủ về quan hệ giữa bệnh nhân và thầy thuốc không được lí tưởng, thường thường tìm không đúng bác sĩ hay bệnh viện (do khí vận của mệnh tạo gây ra, ngay cả danh y cũng biến thành thầy thuốc tầm thường). Hơn nữa, Hóa Kị còn có ý tượng "làm cho rối rắm", "làm phiền", "thong thả, chậm", nên mệnh tạo dễ mắc bệnh mạn tính, cần phải thường xuyên kiểm tra sức khỏe. Vì Hóa Kị còn có ý tượng "mờ ám", "bất minh", nên về bệnh lí, phần nhiều là chí hướng các bệnh không rõ ràng như khối u, ung thư ..</t>
+  </si>
+  <si>
+    <t>Cung điền trạch vốn là đối cung của cung tử nữ, có quan hệ mật thiết với bệnh tật cơ thể; đối với nữ mệnh, trường hợp cung điền trạch có Hóa Kị, ngoại trừ chủ về lo lắng vấn đề sức khỏe lúc mang thai (cần phải thường xuyên kiểm tra định kì, đặc biệt chú ý kiểm tra bệnh phụ khoa nhất là tử cung, buồng trứng).</t>
+  </si>
+  <si>
+    <t>Luận cha mẹ, cung điền trạch là cung vị phúc đức của cung phụ mẫu, thêm vào đó, cung điền trạch có thể xem là cuộc sống gia đình của mệnh tạo; trường hợp cung điền trạch có Hóa Kị, phần nhiều trong đại vận thứ nhất, lúc ấu niên, cuộc sống gia đình của mệnh tạo thường xảy ra rất nhiều vấn đề, thông thường là do hôn nhân của song thân không được hòa hợp làm cho mệnh tạo có tâm trạng bi quan.</t>
+  </si>
+  <si>
+    <t>Tiếp theo trên, cung điền trạch cư ở cung vị thiên di của cung tử nữ, là chủ về cảm giác của con cái đối với gia đình; trường hợp có Hóa Kị, là con cái của mệnh tạo không lạc quan về tương lai của gia đình, trong nhà sẽ thấy tình huống u ám, tuy mệnh tạo muốn tích cực lo cho cuộc sống gia đình (Hóa Kị cũng là "ước muốn"), nhưng đối với con cái, chúng lại thiếu cảm giác ấm áp.</t>
+  </si>
+  <si>
+    <t>Cung điền trạch còn tượng trưng cho hoàn cảnh chung quanh, môi trường mà mệnh tạo tiếp xúc hàng ngày, cho nên cũng có thể xem là môi trường làm việc của mệnh tạo; trường hợp có Hóa Kị, có thể thấy hoàn cảnh môi trường làm việc của mệnh tạo không được lí tưởng, nếu không phải là tài chính có vấn đề, mà là tượng rối loạn, chế độ nhân sự không rõ rệt, hoặc ông chủ ngầm giở quỷ kế.</t>
+  </si>
+  <si>
+    <t>Vì cung điền trạch là đối cung của cung tử nữ, luận ở tầng thâm sâu, tuyến "từ điền" có tính chất đào hoa hưởng lạc; trường hợp cung điền trạch có Hóa Kị, không phải là không có đào hoa, mà một khi xảy ra quan hệ đào hoa thì sẽ dây dưa không dứt, quan hệ đào hoa thường thường sẽ liên quan với người đã kết hôn, có cơ hội rất lớn trở thành nam nữ vai chính trong vở bi kịch tình tay ba.</t>
   </si>
 </sst>
 </file>
@@ -5962,10 +6022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:K1635"/>
+  <dimension ref="A2:M1635"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1177" workbookViewId="0">
-      <selection activeCell="J1178" sqref="J1178"/>
+    <sheetView tabSelected="1" topLeftCell="H1223" workbookViewId="0">
+      <selection activeCell="L1224" sqref="L1224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5974,12 +6034,14 @@
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="56.28515625" customWidth="1"/>
     <col min="5" max="5" width="44.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1"/>
+    <col min="7" max="7" width="49.28515625" customWidth="1"/>
+    <col min="8" max="8" width="38.140625" customWidth="1"/>
+    <col min="9" max="9" width="44.42578125" customWidth="1"/>
     <col min="10" max="10" width="36.7109375" customWidth="1"/>
     <col min="11" max="11" width="46.42578125" customWidth="1"/>
+    <col min="12" max="12" width="42.140625" customWidth="1"/>
+    <col min="13" max="13" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -15395,7 +15457,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="1177" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+    <row r="1177" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A1177" s="1" t="s">
         <v>16</v>
       </c>
@@ -15799,7 +15861,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="1217" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="1217" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A1217" s="1" t="s">
         <v>1214</v>
       </c>
@@ -15810,7 +15872,7 @@
         <v>1777</v>
       </c>
     </row>
-    <row r="1218" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="1218" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1218" s="1" t="s">
         <v>1215</v>
       </c>
@@ -15818,7 +15880,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="1219" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="1219" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1219" s="1" t="s">
         <v>1216</v>
       </c>
@@ -15826,7 +15888,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="1220" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="1220" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1220" s="1" t="s">
         <v>1217</v>
       </c>
@@ -15834,7 +15896,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="1221" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="1221" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1221" s="1" t="s">
         <v>1218</v>
       </c>
@@ -15845,7 +15907,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="1222" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="1222" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1222" s="1" t="s">
         <v>1219</v>
       </c>
@@ -15853,7 +15915,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="1223" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1223" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1223" s="1" t="s">
         <v>1220</v>
       </c>
@@ -15861,23 +15923,83 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="1224" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="1224" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A1224" s="1" t="s">
         <v>1221</v>
       </c>
       <c r="B1224" s="1" t="s">
         <v>1783</v>
       </c>
-    </row>
-    <row r="1225" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="C1224" s="1" t="s">
+        <v>1860</v>
+      </c>
+      <c r="D1224" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="E1224" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="F1224" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="G1224" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="H1224" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="I1224" s="1" t="s">
+        <v>1866</v>
+      </c>
+      <c r="J1224" s="1" t="s">
+        <v>1867</v>
+      </c>
+      <c r="K1224" s="1" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A1225" s="1" t="s">
         <v>1222</v>
       </c>
       <c r="B1225" s="1" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="1226" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="C1225" s="1" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D1225" s="1" t="s">
+        <v>1870</v>
+      </c>
+      <c r="E1225" s="1" t="s">
+        <v>1871</v>
+      </c>
+      <c r="F1225" s="1" t="s">
+        <v>1872</v>
+      </c>
+      <c r="G1225" s="1" t="s">
+        <v>1873</v>
+      </c>
+      <c r="H1225" s="1" t="s">
+        <v>1874</v>
+      </c>
+      <c r="I1225" s="1" t="s">
+        <v>1875</v>
+      </c>
+      <c r="J1225" s="1" t="s">
+        <v>1876</v>
+      </c>
+      <c r="K1225" s="1" t="s">
+        <v>1877</v>
+      </c>
+      <c r="L1225" s="1" t="s">
+        <v>1878</v>
+      </c>
+      <c r="M1225" s="1" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A1226" s="1" t="s">
         <v>1223</v>
       </c>
@@ -15888,7 +16010,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="1227" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="1227" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A1227" s="1" t="s">
         <v>1224</v>
       </c>
@@ -15896,7 +16018,7 @@
         <v>1786</v>
       </c>
     </row>
-    <row r="1228" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="1228" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A1228" s="1" t="s">
         <v>1225</v>
       </c>
@@ -15904,7 +16026,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="1229" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="1229" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1229" s="1" t="s">
         <v>1226</v>
       </c>
@@ -15912,7 +16034,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="1230" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="1230" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A1230" s="1" t="s">
         <v>1227</v>
       </c>
@@ -15920,7 +16042,7 @@
         <v>1789</v>
       </c>
     </row>
-    <row r="1231" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="1231" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A1231" s="1" t="s">
         <v>1228</v>
       </c>
@@ -15928,7 +16050,7 @@
         <v>1789</v>
       </c>
     </row>
-    <row r="1232" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1232" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1232" s="1" t="s">
         <v>1229</v>
       </c>

</xml_diff>